<commit_message>
Adding CAD finger files & Updated Excel Sheet
</commit_message>
<xml_diff>
--- a/Excel Files/Bill Of Materials.xlsx
+++ b/Excel Files/Bill Of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m\Desktop\Projects\EMGingers-control\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB0E42B-E8A1-48EE-8D53-5964B5CA24AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6FAFCD-0F9D-4D97-826F-59AC869B3A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C8C1D8BB-10F7-49BF-8560-67C50CB8DDC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C8C1D8BB-10F7-49BF-8560-67C50CB8DDC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>No</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>Connect wires</t>
+  </si>
+  <si>
+    <t>Worm Gear Motor With encoder</t>
+  </si>
+  <si>
+    <t>Self locking with position data, very useful</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Torque-Reduction-Encoder-Self-locking-Output/dp/B073S65J25</t>
+  </si>
+  <si>
+    <t>Links</t>
   </si>
 </sst>
 </file>
@@ -267,10 +279,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,21 +604,21 @@
   <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="227.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="227.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -632,10 +647,10 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -659,7 +674,7 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -683,7 +698,7 @@
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -707,8 +722,11 @@
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -728,7 +746,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -749,7 +767,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -767,7 +785,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -785,7 +803,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -806,7 +824,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -827,7 +845,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -848,7 +866,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -866,7 +884,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -884,7 +902,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -902,7 +920,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -920,7 +938,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -938,7 +956,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -956,7 +974,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -974,7 +992,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -992,10 +1010,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1013,7 +1031,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1031,7 +1049,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1049,7 +1067,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1067,7 +1085,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1085,7 +1103,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1093,9 +1111,21 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>